<commit_message>
Adding Accessabilty Axe engine support to framework.
</commit_message>
<xml_diff>
--- a/TestScripts/HomePage/ApplicationLogin.xlsx
+++ b/TestScripts/HomePage/ApplicationLogin.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SELENIUM_FW\SeleniumPOM_DD\TestScripts\HomePage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\selenium_project\TestScripts\HomePage\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>